<commit_message>
Changes to manuals and DCT evaluation. Before WO Changes.
</commit_message>
<xml_diff>
--- a/FM/working-status/FM-Status.xlsx
+++ b/FM/working-status/FM-Status.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/camroe/working/RepairServiceManual/FM/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/camroe/working/RepairServiceManual/FM/working-status/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2AE9FD26-9D2C-744F-B612-10F51F322640}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68185516-1947-4B41-8BDF-5C94CB792C85}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="24260" yWindow="-18540" windowWidth="27640" windowHeight="18540" xr2:uid="{6B23032B-54A6-D642-AD6D-9CF5C8532F8E}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="35">
   <si>
     <t>Form</t>
   </si>
@@ -128,6 +127,12 @@
   <si>
     <t>Instructions
 Section 7</t>
+  </si>
+  <si>
+    <t>CAM</t>
+  </si>
+  <si>
+    <t>JEFF!</t>
   </si>
 </sst>
 </file>
@@ -578,7 +583,7 @@
   <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -734,7 +739,9 @@
       <c r="C10" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="1"/>
+      <c r="D10" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -747,7 +754,9 @@
       <c r="C11" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="1"/>
+      <c r="D11" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -790,7 +799,9 @@
       <c r="C14" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="1"/>
+      <c r="D14" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="E14" s="1"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -818,7 +829,9 @@
       <c r="C16" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="1"/>
+      <c r="D16" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="E16" s="1"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -861,7 +874,9 @@
       <c r="C19" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D19" s="1"/>
+      <c r="D19" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="E19" s="1"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -874,7 +889,9 @@
       <c r="C20" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D20" s="1"/>
+      <c r="D20" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="E20" s="1"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -887,7 +904,9 @@
       <c r="C21" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D21" s="1"/>
+      <c r="D21" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="E21" s="1"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -900,7 +919,9 @@
       <c r="C22" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D22" s="1"/>
+      <c r="D22" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="E22" s="1"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -913,7 +934,9 @@
       <c r="C23" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D23" s="1"/>
+      <c r="D23" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="E23" s="1"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -926,7 +949,9 @@
       <c r="C24" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D24" s="1"/>
+      <c r="D24" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="E24" s="1"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -939,7 +964,9 @@
       <c r="C25" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D25" s="1"/>
+      <c r="D25" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="E25" s="1"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>